<commit_message>
Ready line & split billing avis scripts
</commit_message>
<xml_diff>
--- a/AVIS/TestData/AVIS_GUITestData_ReadyLine_Regression.xlsx
+++ b/AVIS/TestData/AVIS_GUITestData_ReadyLine_Regression.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GUI_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_Clone\ABG\AVIS\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView tabRatio="859" windowHeight="2070" windowWidth="20925" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20925" windowHeight="2070" tabRatio="859"/>
   </bookViews>
   <sheets>
-    <sheet name="INPUT_DATA" r:id="rId1" sheetId="2"/>
-    <sheet name="INPUT_DATA_UAT_2" r:id="rId2" sheetId="1"/>
+    <sheet name="INPUT_DATA" sheetId="2" r:id="rId1"/>
+    <sheet name="INPUT_DATA_UAT_2" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">INPUT_DATA!$A$1:$BY$33</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">INPUT_DATA_UAT_2!$A$1:$BY$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">INPUT_DATA!$A$1:$BY$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">INPUT_DATA_UAT_2!$A$1:$BY$33</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="218">
   <si>
     <t>EXECUTE</t>
   </si>
@@ -665,26 +665,25 @@
     <t>N</t>
   </si>
   <si>
-    <t>https://wizardgui-uat.avisbudget.com/wizardgui/ui/wizard.jsf?mnemonic=</t>
-  </si>
-  <si>
     <t>https://wizardgui-uat.avisbudget.com/wizardgui2/ui/wizard.jsf?mnemonic=</t>
   </si>
   <si>
-    <t>Avis0909#</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1 items found. </t>
   </si>
   <si>
     <t xml:space="preserve"> 0 items found. </t>
+  </si>
+  <si>
+    <t>Avis2018#</t>
+  </si>
+  <si>
+    <t>https://uat.ccrgservices.com/wizardgui/ui/wizard.jsf?mnemonic=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -776,84 +775,87 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="3" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="3" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="3" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="4" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="5" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -870,10 +872,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -908,7 +910,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -943,7 +945,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1037,21 +1039,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1068,7 +1070,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1120,57 +1122,53 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:BZ33"/>
+  <dimension ref="A1:BY33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0" zoomScale="96" zoomScaleNormal="96">
-      <selection activeCell="BW1" sqref="BW1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.25" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="66.125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="56.75" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" hidden="true" width="92.375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" hidden="true" width="53.875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="14.875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="28" width="17.625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="14" max="21" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="23" max="31" bestFit="true" customWidth="true" width="12.625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="13.625" collapsed="true"/>
-    <col min="33" max="34" bestFit="true" customWidth="true" width="10.875" collapsed="true"/>
-    <col min="35" max="41" bestFit="true" customWidth="true" width="10.875" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="11.875" collapsed="true"/>
-    <col min="43" max="48" bestFit="true" customWidth="true" width="9.5" collapsed="true"/>
-    <col min="50" max="51" bestFit="true" customWidth="true" width="9.5" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="10.375" collapsed="true"/>
-    <col min="53" max="61" bestFit="true" customWidth="true" width="14.625" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" width="15.625" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="11.25" collapsed="true"/>
-    <col min="64" max="73" bestFit="true" customWidth="true" width="15.375" collapsed="true"/>
-    <col min="74" max="74" bestFit="true" customWidth="true" width="16.375" collapsed="true"/>
-    <col min="75" max="75" bestFit="true" customWidth="true" width="16.125" collapsed="true"/>
-    <col min="76" max="76" bestFit="true" customWidth="true" width="28.875" collapsed="true"/>
-    <col min="77" max="77" bestFit="true" customWidth="true" width="21.75" collapsed="true"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="66.125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="56.75" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="92.375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="53.875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.625" style="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="21" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="31" width="12.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="41" width="10.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="48" width="9.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="51" width="9.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="61" width="14.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="11.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="73" width="15.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="16.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="28.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="77" max="77" width="21.75" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -1403,7 +1401,7 @@
         <v>85</v>
       </c>
     </row>
-    <row ht="15" r="2" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -1411,7 +1409,7 @@
         <v>78</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>1</v>
+        <v>212</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>14</v>
@@ -1425,14 +1423,14 @@
       <c r="G2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>213</v>
+      <c r="H2" s="17" t="s">
+        <v>217</v>
       </c>
       <c r="I2" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K2" s="25" t="s">
         <v>88</v>
@@ -1503,12 +1501,12 @@
       <c r="BU2" s="6"/>
       <c r="BV2" s="6"/>
       <c r="BW2" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="BX2" s="12"/>
       <c r="BY2" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="3" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1516,7 +1514,7 @@
         <v>79</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>14</v>
@@ -1531,19 +1529,19 @@
         <v>13</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I3" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K3" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="L3" s="6">
-        <v>0</v>
+      <c r="L3" s="29" t="s">
+        <v>77</v>
       </c>
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
@@ -1611,7 +1609,7 @@
       <c r="BX3" s="12"/>
       <c r="BY3" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="4" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
@@ -1619,7 +1617,7 @@
         <v>89</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>14</v>
@@ -1634,19 +1632,19 @@
         <v>13</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I4" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K4" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="L4" s="6">
-        <v>1</v>
+      <c r="L4" s="29" t="s">
+        <v>78</v>
       </c>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
@@ -1714,7 +1712,7 @@
       <c r="BX4" s="12"/>
       <c r="BY4" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="5" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>10</v>
       </c>
@@ -1722,7 +1720,7 @@
         <v>90</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>14</v>
@@ -1737,19 +1735,19 @@
         <v>13</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I5" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K5" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="L5" s="6">
-        <v>2</v>
+      <c r="L5" s="29" t="s">
+        <v>79</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
@@ -1817,7 +1815,7 @@
       <c r="BX5" s="12"/>
       <c r="BY5" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="6" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
@@ -1825,7 +1823,7 @@
         <v>91</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>14</v>
@@ -1840,19 +1838,19 @@
         <v>13</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I6" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K6" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="L6" s="6">
-        <v>3</v>
+      <c r="L6" s="29" t="s">
+        <v>89</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -1920,7 +1918,7 @@
       <c r="BX6" s="12"/>
       <c r="BY6" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="7" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
@@ -1928,7 +1926,7 @@
         <v>92</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>14</v>
@@ -1943,19 +1941,19 @@
         <v>13</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I7" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K7" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="L7" s="6">
-        <v>4</v>
+      <c r="L7" s="29" t="s">
+        <v>90</v>
       </c>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
@@ -2023,7 +2021,7 @@
       <c r="BX7" s="6"/>
       <c r="BY7" s="6"/>
     </row>
-    <row ht="15" r="8" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
@@ -2031,7 +2029,7 @@
         <v>93</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>1</v>
+        <v>212</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>14</v>
@@ -2046,13 +2044,13 @@
         <v>13</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I8" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K8" s="25" t="s">
         <v>88</v>
@@ -2123,12 +2121,12 @@
       <c r="BU8" s="12"/>
       <c r="BV8" s="12"/>
       <c r="BW8" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="BX8" s="6"/>
       <c r="BY8" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="9" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>10</v>
       </c>
@@ -2136,7 +2134,7 @@
         <v>76</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>14</v>
@@ -2151,19 +2149,19 @@
         <v>13</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I9" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K9" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="L9" s="6">
-        <v>6</v>
+      <c r="L9" s="29" t="s">
+        <v>92</v>
       </c>
       <c r="M9" s="12"/>
       <c r="N9" s="12"/>
@@ -2231,7 +2229,7 @@
       <c r="BX9" s="6"/>
       <c r="BY9" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="10" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>10</v>
       </c>
@@ -2239,7 +2237,7 @@
         <v>94</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>14</v>
@@ -2254,19 +2252,19 @@
         <v>13</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I10" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K10" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="L10" s="6">
-        <v>7</v>
+      <c r="L10" s="29" t="s">
+        <v>93</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
@@ -2334,7 +2332,7 @@
       <c r="BX10" s="6"/>
       <c r="BY10" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="11" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>10</v>
       </c>
@@ -2342,7 +2340,7 @@
         <v>95</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>14</v>
@@ -2357,19 +2355,19 @@
         <v>13</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I11" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K11" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="L11" s="6">
-        <v>8</v>
+      <c r="L11" s="29" t="s">
+        <v>76</v>
       </c>
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
@@ -2437,7 +2435,7 @@
       <c r="BX11" s="6"/>
       <c r="BY11" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="12" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
@@ -2445,7 +2443,7 @@
         <v>96</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>14</v>
@@ -2460,19 +2458,19 @@
         <v>13</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I12" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K12" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="L12" s="6">
-        <v>9</v>
+      <c r="L12" s="29" t="s">
+        <v>94</v>
       </c>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
@@ -2540,7 +2538,7 @@
       <c r="BX12" s="6"/>
       <c r="BY12" s="6"/>
     </row>
-    <row ht="15" r="13" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>10</v>
       </c>
@@ -2548,7 +2546,7 @@
         <v>97</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>1</v>
+        <v>212</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>14</v>
@@ -2563,13 +2561,13 @@
         <v>13</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I13" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K13" s="25" t="s">
         <v>88</v>
@@ -2640,12 +2638,12 @@
       <c r="BU13" s="12"/>
       <c r="BV13" s="12"/>
       <c r="BW13" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="BX13" s="6"/>
       <c r="BY13" s="6"/>
     </row>
-    <row ht="15" r="14" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>10</v>
       </c>
@@ -2653,7 +2651,7 @@
         <v>98</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>1</v>
+        <v>212</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>14</v>
@@ -2668,13 +2666,13 @@
         <v>13</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I14" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K14" s="25" t="s">
         <v>88</v>
@@ -2745,12 +2743,12 @@
       <c r="BU14" s="12"/>
       <c r="BV14" s="12"/>
       <c r="BW14" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="BX14" s="6"/>
       <c r="BY14" s="6"/>
     </row>
-    <row ht="15" r="15" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>10</v>
       </c>
@@ -2758,7 +2756,7 @@
         <v>99</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>1</v>
+        <v>212</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>14</v>
@@ -2773,13 +2771,13 @@
         <v>13</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I15" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K15" s="25" t="s">
         <v>88</v>
@@ -2850,12 +2848,12 @@
       <c r="BU15" s="12"/>
       <c r="BV15" s="12"/>
       <c r="BW15" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="BX15" s="6"/>
       <c r="BY15" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="16" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>10</v>
       </c>
@@ -2878,13 +2876,13 @@
         <v>13</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K16" s="25" t="s">
         <v>88</v>
@@ -3056,7 +3054,7 @@
       <c r="BX16" s="12"/>
       <c r="BY16" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="17" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>10</v>
       </c>
@@ -3079,13 +3077,13 @@
         <v>13</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I17" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K17" s="25" t="s">
         <v>88</v>
@@ -3161,7 +3159,7 @@
       <c r="BX17" s="12"/>
       <c r="BY17" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="18" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>10</v>
       </c>
@@ -3184,13 +3182,13 @@
         <v>13</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I18" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K18" s="26" t="s">
         <v>36</v>
@@ -3264,7 +3262,7 @@
       <c r="BX18" s="12"/>
       <c r="BY18" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="19" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>10</v>
       </c>
@@ -3287,13 +3285,13 @@
         <v>13</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I19" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J19" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K19" s="24" t="s">
         <v>37</v>
@@ -3367,7 +3365,7 @@
       <c r="BX19" s="12"/>
       <c r="BY19" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="20" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>10</v>
       </c>
@@ -3390,13 +3388,13 @@
         <v>13</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I20" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K20" s="24" t="s">
         <v>38</v>
@@ -3470,7 +3468,7 @@
       <c r="BX20" s="12"/>
       <c r="BY20" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="21" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>10</v>
       </c>
@@ -3493,13 +3491,13 @@
         <v>13</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I21" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J21" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K21" s="24" t="s">
         <v>39</v>
@@ -3573,7 +3571,7 @@
       <c r="BX21" s="12"/>
       <c r="BY21" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="22" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>10</v>
       </c>
@@ -3596,13 +3594,13 @@
         <v>13</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I22" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K22" s="24" t="s">
         <v>40</v>
@@ -3676,7 +3674,7 @@
       <c r="BX22" s="12"/>
       <c r="BY22" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="23" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>10</v>
       </c>
@@ -3699,13 +3697,13 @@
         <v>13</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I23" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J23" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K23" s="24" t="s">
         <v>41</v>
@@ -3779,7 +3777,7 @@
       <c r="BX23" s="6"/>
       <c r="BY23" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="24" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>10</v>
       </c>
@@ -3802,13 +3800,13 @@
         <v>13</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I24" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K24" s="24" t="s">
         <v>42</v>
@@ -3882,7 +3880,7 @@
       <c r="BX24" s="6"/>
       <c r="BY24" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="25" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>10</v>
       </c>
@@ -3905,13 +3903,13 @@
         <v>13</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I25" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K25" s="24" t="s">
         <v>43</v>
@@ -3985,7 +3983,7 @@
       <c r="BX25" s="6"/>
       <c r="BY25" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="26" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>10</v>
       </c>
@@ -4008,13 +4006,13 @@
         <v>13</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I26" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K26" s="24" t="s">
         <v>44</v>
@@ -4088,7 +4086,7 @@
       <c r="BX26" s="6"/>
       <c r="BY26" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="27" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>10</v>
       </c>
@@ -4111,13 +4109,13 @@
         <v>13</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I27" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K27" s="24" t="s">
         <v>45</v>
@@ -4191,7 +4189,7 @@
       <c r="BX27" s="6"/>
       <c r="BY27" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="28" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>10</v>
       </c>
@@ -4214,13 +4212,13 @@
         <v>13</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I28" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K28" s="24" t="s">
         <v>46</v>
@@ -4294,7 +4292,7 @@
       <c r="BX28" s="6"/>
       <c r="BY28" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="29" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>10</v>
       </c>
@@ -4317,13 +4315,13 @@
         <v>13</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I29" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K29" s="24" t="s">
         <v>47</v>
@@ -4397,7 +4395,7 @@
       <c r="BX29" s="6"/>
       <c r="BY29" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="30" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>10</v>
       </c>
@@ -4420,13 +4418,13 @@
         <v>13</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I30" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J30" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K30" s="24" t="s">
         <v>48</v>
@@ -4500,7 +4498,7 @@
       <c r="BX30" s="6"/>
       <c r="BY30" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="31" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>10</v>
       </c>
@@ -4523,13 +4521,13 @@
         <v>13</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J31" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K31" s="24" t="s">
         <v>49</v>
@@ -4603,7 +4601,7 @@
       <c r="BX31" s="6"/>
       <c r="BY31" s="6"/>
     </row>
-    <row hidden="1" ht="15" r="32" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>10</v>
       </c>
@@ -4626,13 +4624,13 @@
         <v>13</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I32" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J32" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K32" s="24" t="s">
         <v>37</v>
@@ -4804,7 +4802,7 @@
       <c r="BX32" s="12"/>
       <c r="BY32" s="12"/>
     </row>
-    <row hidden="1" ht="15" r="33" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>10</v>
       </c>
@@ -4827,13 +4825,13 @@
         <v>13</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I33" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J33" s="24" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K33" s="24" t="s">
         <v>39</v>
@@ -4917,58 +4915,58 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FX141"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:FW141"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="20.625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="14.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="12.25" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="66.125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="60.625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="92.375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="62.625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="10.875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="17.625" collapsed="true"/>
-    <col min="13" max="22" customWidth="true" style="1" width="8.875" collapsed="true"/>
-    <col min="23" max="31" customWidth="true" style="1" width="8.625" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" style="1" width="10.75" collapsed="true"/>
-    <col min="33" max="41" customWidth="true" style="1" width="6.875" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="7.875" collapsed="true"/>
-    <col min="43" max="51" customWidth="true" style="1" width="5.375" collapsed="true"/>
-    <col min="52" max="52" customWidth="true" style="1" width="8.375" collapsed="true"/>
-    <col min="53" max="61" customWidth="true" style="1" width="10.625" collapsed="true"/>
-    <col min="62" max="62" customWidth="true" style="1" width="13.75" collapsed="true"/>
-    <col min="63" max="63" customWidth="true" style="1" width="15.5" collapsed="true"/>
-    <col min="64" max="64" customWidth="true" style="1" width="20.625" collapsed="true"/>
-    <col min="65" max="65" customWidth="true" style="1" width="24.875" collapsed="true"/>
-    <col min="66" max="66" customWidth="true" style="1" width="25.0" collapsed="true"/>
-    <col min="67" max="67" customWidth="true" style="1" width="24.25" collapsed="true"/>
-    <col min="68" max="68" customWidth="true" style="1" width="24.875" collapsed="true"/>
-    <col min="69" max="69" customWidth="true" style="1" width="25.0" collapsed="true"/>
-    <col min="70" max="70" customWidth="true" style="1" width="24.25" collapsed="true"/>
-    <col min="71" max="71" customWidth="true" style="1" width="24.875" collapsed="true"/>
-    <col min="72" max="72" customWidth="true" style="1" width="25.0" collapsed="true"/>
-    <col min="73" max="74" customWidth="true" style="1" width="24.25" collapsed="true"/>
-    <col min="75" max="75" customWidth="true" style="1" width="16.875" collapsed="true"/>
-    <col min="76" max="76" customWidth="true" style="1" width="33.875" collapsed="true"/>
-    <col min="77" max="77" customWidth="true" style="1" width="67.25" collapsed="true"/>
-    <col min="78" max="16384" style="2" width="9.125" collapsed="true"/>
+    <col min="1" max="1" width="20.625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.25" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="66.125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="60.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="92.375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="62.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="22" width="8.875" style="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="31" width="8.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="10.75" style="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="41" width="6.875" style="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="7.875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="51" width="5.375" style="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="8.375" style="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="61" width="10.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="13.75" style="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="15.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="20.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="24.875" style="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="25" style="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="24.25" style="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="24.875" style="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="25" style="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="24.25" style="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="24.875" style="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="25" style="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="74" width="24.25" style="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="16.875" style="1" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="33.875" style="1" customWidth="1" collapsed="1"/>
+    <col min="77" max="77" width="67.25" style="1" customWidth="1" collapsed="1"/>
+    <col min="78" max="16384" width="9.125" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="12.75" r="1" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:179" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -5303,7 +5301,7 @@
       <c r="FV1" s="4"/>
       <c r="FW1" s="4"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="2" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -5326,7 +5324,7 @@
         <v>13</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>5</v>
@@ -5516,7 +5514,7 @@
       <c r="FV2" s="5"/>
       <c r="FW2" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="3" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -5539,7 +5537,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I3" s="17" t="s">
         <v>5</v>
@@ -5721,7 +5719,7 @@
       <c r="FV3" s="5"/>
       <c r="FW3" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="4" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
@@ -5744,7 +5742,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>5</v>
@@ -5926,7 +5924,7 @@
       <c r="FV4" s="5"/>
       <c r="FW4" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="5" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>10</v>
       </c>
@@ -5949,7 +5947,7 @@
         <v>13</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>5</v>
@@ -6131,7 +6129,7 @@
       <c r="FV5" s="5"/>
       <c r="FW5" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="6" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
@@ -6154,7 +6152,7 @@
         <v>13</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>5</v>
@@ -6336,7 +6334,7 @@
       <c r="FV6" s="5"/>
       <c r="FW6" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="7" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
@@ -6359,7 +6357,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>5</v>
@@ -6541,7 +6539,7 @@
       <c r="FV7" s="5"/>
       <c r="FW7" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="8" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
@@ -6564,7 +6562,7 @@
         <v>13</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>5</v>
@@ -6746,7 +6744,7 @@
       <c r="FV8" s="5"/>
       <c r="FW8" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="9" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>10</v>
       </c>
@@ -6769,7 +6767,7 @@
         <v>13</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I9" s="17" t="s">
         <v>5</v>
@@ -6951,7 +6949,7 @@
       <c r="FV9" s="5"/>
       <c r="FW9" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="10" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>10</v>
       </c>
@@ -6974,7 +6972,7 @@
         <v>13</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>5</v>
@@ -7156,7 +7154,7 @@
       <c r="FV10" s="5"/>
       <c r="FW10" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="11" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>10</v>
       </c>
@@ -7179,7 +7177,7 @@
         <v>13</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>5</v>
@@ -7361,7 +7359,7 @@
       <c r="FV11" s="5"/>
       <c r="FW11" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="12" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
@@ -7384,7 +7382,7 @@
         <v>13</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>5</v>
@@ -7566,7 +7564,7 @@
       <c r="FV12" s="5"/>
       <c r="FW12" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="13" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>10</v>
       </c>
@@ -7589,7 +7587,7 @@
         <v>13</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I13" s="17" t="s">
         <v>5</v>
@@ -7771,7 +7769,7 @@
       <c r="FV13" s="5"/>
       <c r="FW13" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="14" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>10</v>
       </c>
@@ -7794,7 +7792,7 @@
         <v>13</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>5</v>
@@ -7976,7 +7974,7 @@
       <c r="FV14" s="5"/>
       <c r="FW14" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="15" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>10</v>
       </c>
@@ -7999,7 +7997,7 @@
         <v>13</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>5</v>
@@ -8181,7 +8179,7 @@
       <c r="FV15" s="5"/>
       <c r="FW15" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="16" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>10</v>
       </c>
@@ -8204,7 +8202,7 @@
         <v>13</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>5</v>
@@ -8500,7 +8498,7 @@
       <c r="FV16" s="5"/>
       <c r="FW16" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="17" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>10</v>
       </c>
@@ -8523,7 +8521,7 @@
         <v>13</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I17" s="17" t="s">
         <v>5</v>
@@ -8707,7 +8705,7 @@
       <c r="FV17" s="5"/>
       <c r="FW17" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="18" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>10</v>
       </c>
@@ -8730,7 +8728,7 @@
         <v>13</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I18" s="17" t="s">
         <v>5</v>
@@ -8916,7 +8914,7 @@
       <c r="FV18" s="5"/>
       <c r="FW18" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="19" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>10</v>
       </c>
@@ -8939,7 +8937,7 @@
         <v>13</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I19" s="17" t="s">
         <v>5</v>
@@ -9123,7 +9121,7 @@
       <c r="FV19" s="5"/>
       <c r="FW19" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="20" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>10</v>
       </c>
@@ -9146,7 +9144,7 @@
         <v>13</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I20" s="17" t="s">
         <v>5</v>
@@ -9330,7 +9328,7 @@
       <c r="FV20" s="5"/>
       <c r="FW20" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="21" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>10</v>
       </c>
@@ -9353,7 +9351,7 @@
         <v>13</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I21" s="17" t="s">
         <v>5</v>
@@ -9537,7 +9535,7 @@
       <c r="FV21" s="5"/>
       <c r="FW21" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="22" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>10</v>
       </c>
@@ -9560,7 +9558,7 @@
         <v>13</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I22" s="17" t="s">
         <v>5</v>
@@ -9744,7 +9742,7 @@
       <c r="FV22" s="5"/>
       <c r="FW22" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="23" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>10</v>
       </c>
@@ -9767,7 +9765,7 @@
         <v>13</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I23" s="17" t="s">
         <v>5</v>
@@ -9951,7 +9949,7 @@
       <c r="FV23" s="5"/>
       <c r="FW23" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="24" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>10</v>
       </c>
@@ -9974,7 +9972,7 @@
         <v>13</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I24" s="17" t="s">
         <v>5</v>
@@ -10158,7 +10156,7 @@
       <c r="FV24" s="5"/>
       <c r="FW24" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="25" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>10</v>
       </c>
@@ -10181,7 +10179,7 @@
         <v>13</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I25" s="17" t="s">
         <v>5</v>
@@ -10365,7 +10363,7 @@
       <c r="FV25" s="5"/>
       <c r="FW25" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="26" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>10</v>
       </c>
@@ -10388,7 +10386,7 @@
         <v>13</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I26" s="17" t="s">
         <v>5</v>
@@ -10572,7 +10570,7 @@
       <c r="FV26" s="5"/>
       <c r="FW26" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="27" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>10</v>
       </c>
@@ -10595,7 +10593,7 @@
         <v>13</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>5</v>
@@ -10779,7 +10777,7 @@
       <c r="FV27" s="5"/>
       <c r="FW27" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="28" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>10</v>
       </c>
@@ -10802,7 +10800,7 @@
         <v>13</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I28" s="17" t="s">
         <v>5</v>
@@ -10986,7 +10984,7 @@
       <c r="FV28" s="5"/>
       <c r="FW28" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="29" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>10</v>
       </c>
@@ -11009,7 +11007,7 @@
         <v>13</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I29" s="17" t="s">
         <v>5</v>
@@ -11193,7 +11191,7 @@
       <c r="FV29" s="5"/>
       <c r="FW29" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="30" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>10</v>
       </c>
@@ -11216,7 +11214,7 @@
         <v>13</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I30" s="17" t="s">
         <v>5</v>
@@ -11400,7 +11398,7 @@
       <c r="FV30" s="5"/>
       <c r="FW30" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="31" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>10</v>
       </c>
@@ -11423,7 +11421,7 @@
         <v>13</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I31" s="17" t="s">
         <v>5</v>
@@ -11607,7 +11605,7 @@
       <c r="FV31" s="5"/>
       <c r="FW31" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="32" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>10</v>
       </c>
@@ -11630,7 +11628,7 @@
         <v>13</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I32" s="17" t="s">
         <v>5</v>
@@ -11928,7 +11926,7 @@
       <c r="FV32" s="5"/>
       <c r="FW32" s="5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="33" s="3" spans="1:179" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>10</v>
       </c>
@@ -11951,7 +11949,7 @@
         <v>13</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I33" s="17" t="s">
         <v>5</v>
@@ -20346,7 +20344,7 @@
       <c r="CK141" s="10"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;"Arial,Bold Italic"&amp;14Accenture Confidential</oddFooter>

</xml_diff>